<commit_message>
with corrections and workflow Add an Applicant to Period
</commit_message>
<xml_diff>
--- a/framework/utils/testStages.xlsx
+++ b/framework/utils/testStages.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stages" sheetId="1" r:id="rId1"/>
-    <sheet name="Programs" sheetId="3" r:id="rId2"/>
+    <sheet name="Periods" sheetId="4" r:id="rId2"/>
+    <sheet name="Programs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -82,6 +83,39 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>initialDate</t>
+  </si>
+  <si>
+    <t>period1program1</t>
+  </si>
+  <si>
+    <t>period2program1</t>
+  </si>
+  <si>
+    <t>period3program1</t>
+  </si>
+  <si>
+    <t>programID</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>2014-08-31</t>
+  </si>
+  <si>
+    <t>2014-08-29</t>
+  </si>
+  <si>
+    <t>2014-08-28</t>
   </si>
 </sst>
 </file>
@@ -117,9 +151,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -451,8 +487,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>